<commit_message>
redaction of company name
</commit_message>
<xml_diff>
--- a/documents/Evaluation.xlsx
+++ b/documents/Evaluation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.dilley\development\evaluation\evaluation\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.dilley\development\evaluation\evaluation_2\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA5C1BC2-9228-40D6-B8AE-B5CA75FA992B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F3B4023-35BF-4E11-BC87-E45C0EB9543B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25800" yWindow="3750" windowWidth="25800" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-50760" yWindow="5445" windowWidth="25800" windowHeight="18450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Criteria</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Experience</t>
   </si>
   <si>
-    <t>Price</t>
-  </si>
-  <si>
     <t>Technical Proposal</t>
   </si>
   <si>
@@ -52,6 +49,18 @@
   </si>
   <si>
     <t>References</t>
+  </si>
+  <si>
+    <t>at least 10 years is acceptable</t>
+  </si>
+  <si>
+    <t>a high score will be given for the offer to provide references upon contact, no comment is unacceptable</t>
+  </si>
+  <si>
+    <t>alignment with a standard is expected</t>
+  </si>
+  <si>
+    <t>Quality and OHS Policies</t>
   </si>
 </sst>
 </file>
@@ -386,7 +395,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -397,7 +406,7 @@
     <col min="4" max="4" width="17.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -416,12 +425,14 @@
         <v>4</v>
       </c>
       <c r="B2" s="2">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -431,35 +442,38 @@
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="2">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="2">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2">
         <v>10</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
compliance table tested and refined
</commit_message>
<xml_diff>
--- a/documents/Evaluation.xlsx
+++ b/documents/Evaluation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.dilley\development\evaluation\evaluation_2\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F3B4023-35BF-4E11-BC87-E45C0EB9543B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6536D89-9E87-43DD-93C1-C0994E6F57B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-50760" yWindow="5445" windowWidth="25800" windowHeight="18450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-51540" yWindow="3900" windowWidth="25800" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>Criteria</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Experience</t>
   </si>
   <si>
-    <t>Technical Proposal</t>
-  </si>
-  <si>
     <t>Timeline</t>
   </si>
   <si>
@@ -61,6 +58,30 @@
   </si>
   <si>
     <t>Quality and OHS Policies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Technical </t>
+  </si>
+  <si>
+    <t>Code of Conduct</t>
+  </si>
+  <si>
+    <t>Y/N</t>
+  </si>
+  <si>
+    <t>Insurance</t>
+  </si>
+  <si>
+    <t>Contract terms</t>
+  </si>
+  <si>
+    <t>Conflict of Interest</t>
+  </si>
+  <si>
+    <t>Governance</t>
+  </si>
+  <si>
+    <t>Human Rights</t>
   </si>
 </sst>
 </file>
@@ -392,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -403,7 +424,7 @@
     <col min="1" max="1" width="15.44140625" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
     <col min="3" max="3" width="19.21875" customWidth="1"/>
-    <col min="4" max="4" width="17.5546875" customWidth="1"/>
+    <col min="4" max="4" width="49.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -429,12 +450,12 @@
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2">
         <v>30</v>
@@ -444,7 +465,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2">
         <v>15</v>
@@ -454,25 +475,73 @@
     </row>
     <row r="5" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2">
         <v>10</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2">
         <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sub criteria and comments now being evaluated
</commit_message>
<xml_diff>
--- a/documents/Evaluation.xlsx
+++ b/documents/Evaluation.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.dilley\development\evaluation\evaluation_2\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6536D89-9E87-43DD-93C1-C0994E6F57B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{158CF125-67D0-4C17-98E2-A1B4F3A6A75B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51540" yWindow="3900" windowWidth="25800" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25800" yWindow="3750" windowWidth="25800" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$11</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>Criteria</t>
   </si>
@@ -33,9 +36,6 @@
     <t>Weighting (%)</t>
   </si>
   <si>
-    <t>Score (out of 10)</t>
-  </si>
-  <si>
     <t>Comments</t>
   </si>
   <si>
@@ -82,6 +82,27 @@
   </si>
   <si>
     <t>Human Rights</t>
+  </si>
+  <si>
+    <t>score less than 2 if no timeline given</t>
+  </si>
+  <si>
+    <t>organisational capacity</t>
+  </si>
+  <si>
+    <t>delivery of similar services</t>
+  </si>
+  <si>
+    <t>specialist knowledge &amp; experise related to the services requested</t>
+  </si>
+  <si>
+    <t>water industry or related sectors experience</t>
+  </si>
+  <si>
+    <t>key personnel proposed to provide the service</t>
+  </si>
+  <si>
+    <t>higher score if the key personnel are named and background information provided</t>
   </si>
 </sst>
 </file>
@@ -125,13 +146,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -413,21 +437,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.44140625" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="3" max="3" width="19.21875" customWidth="1"/>
-    <col min="4" max="4" width="49.88671875" customWidth="1"/>
+    <col min="3" max="3" width="49.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -437,114 +460,147 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
       </c>
       <c r="B2" s="2">
         <v>35</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2">
+        <v>30</v>
+      </c>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2">
+        <v>15</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="2">
+        <v>10</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+    <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2">
+        <v>10</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="2">
-        <v>30</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="2">
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2">
-        <v>10</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="2">
-        <v>10</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="B16" t="s">
         <v>12</v>
       </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" t="s">
-        <v>13</v>
+      <c r="B18" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C11" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
scoring at the sub criteria level built into the evaluation matrix
</commit_message>
<xml_diff>
--- a/documents/Evaluation.xlsx
+++ b/documents/Evaluation.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.dilley\development\evaluation\evaluation_2\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{158CF125-67D0-4C17-98E2-A1B4F3A6A75B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D55D106-9322-44F5-9016-BEF5E1B14AD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25800" yWindow="3750" windowWidth="25800" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-50640" yWindow="4350" windowWidth="25800" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$12</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>Criteria</t>
   </si>
@@ -48,9 +48,6 @@
     <t>References</t>
   </si>
   <si>
-    <t>at least 10 years is acceptable</t>
-  </si>
-  <si>
     <t>a high score will be given for the offer to provide references upon contact, no comment is unacceptable</t>
   </si>
   <si>
@@ -102,15 +99,428 @@
     <t>key personnel proposed to provide the service</t>
   </si>
   <si>
-    <t>higher score if the key personnel are named and background information provided</t>
+    <t>previous work at Wannon Water</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">9/10 or above: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Multiple successful past engagements with demonstrated positive impact and strong ongoing relationships
+7/10 or above: At least one significant past engagement with clear, documented results
+5/10 or above: Some informal or indirect involvement, such as subcontracting experience with no direct engagement
+Less than 5/10: No prior engagement or only a proposed future partnership,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">
+9/10 or above: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Strong, well-documented organizational structure with defined roles, dedicated resources, and ability to scale rapidly for the project
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">7/10 or above: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Sufficient capacity to deliver, with some minor gaps in role definition or scalability, 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>5/10 or above:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Limited evidence of a structured approach to project resourcing or ability to handle complexity, 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Less than 5/10: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">No clear details on team structure, resourcing, or capability to deliver at scale, </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">9/10 or above: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Proven history of delivering identical services to organizations of comparable size and complexity, with clear examples and results,
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+7/10 or above: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Strong track record of delivering services that are similar in scope or function, but with minor differences, 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">5/10 or above: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Some relevant experience in related service areas, but limited direct alignment with the required services, 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Less than 5/10: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">No clear evidence of delivering comparable services,  </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">9/10 or above: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Deep subject matter expertise, backed by qualifications, accreditations, and demonstrable real-world application, 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">7/10 or above: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Demonstrates competency and relevant knowledge, but may lack specific certifications or direct application, 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">5/10 or above: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">General industry knowledge without strong specialization or applied expertise in the requested area, 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Less than 5/10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: No clear expertise demonstrated or only general awareness, 
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">9/10 or above: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Extensive experience within the water industry, with deep knowledge of sector-specific regulations, processes, and challenges, 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">7/10 or above: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Strong experience in closely related industries (e,g,, utilities, infrastructure) with some exposure to the water sector, 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">5/10 or above: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Limited but relevant experience in regulatory or public-sector work that could translate into water industry needs, 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Less than 5/10: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">No relevant water industry or closely related sector experience, </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">9/10 or above: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Named individuals with well-documented qualifications, deep experience, and directly relevant project involvement, 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">7/10 or above: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Key personnel identified with relevant expertise, but lacking detail on experience or project involvement, 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">5/10 or above: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Some mention of key personnel but lacking specific qualifications, named individuals, or role clarity, 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Less than 5/10: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">No mention of key personnel or vague/non-detailed references to available staff, </t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -121,9 +531,8 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -146,9 +555,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -156,6 +565,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -437,17 +855,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="3" max="3" width="49.88671875" customWidth="1"/>
+    <col min="3" max="3" width="49.88671875" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -462,145 +880,160 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="4">
         <v>35</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="207.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="193.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="207.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="193.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="193.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="4">
+        <v>30</v>
+      </c>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="4">
+        <v>15</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="4">
+        <v>10</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+    <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="4">
         <v>10</v>
       </c>
-      <c r="B8" s="2">
-        <v>30</v>
-      </c>
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="2">
-        <v>15</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="2">
-        <v>10</v>
-      </c>
-      <c r="C10" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="2">
-        <v>10</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C11" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:C12" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>